<commit_message>
docs: add updated version of the Burndownchart
</commit_message>
<xml_diff>
--- a/docs/BurnDownChart.xlsx
+++ b/docs/BurnDownChart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valkalin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valkalin\Documents\306\VJLF-306\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Status</t>
   </si>
@@ -38,22 +38,6 @@
     <t>Membre</t>
   </si>
   <si>
-    <t>Jour 1</t>
-  </si>
-  <si>
-    <t>Jour 2</t>
-  </si>
-  <si>
-    <t>Jour 3</t>
-  </si>
-  <si>
-    <t>Jour 4</t>
-  </si>
-  <si>
-    <t>Sprint 
-Review</t>
-  </si>
-  <si>
     <t>Story points estimés</t>
   </si>
   <si>
@@ -123,7 +107,25 @@
     <t>Détails d'un consommables</t>
   </si>
   <si>
-    <t>Jour 5</t>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Sprint 5</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Valentin, Lazar</t>
   </si>
 </sst>
 </file>
@@ -189,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -229,11 +231,120 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -263,7 +374,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -274,34 +385,66 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="23" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="23" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="23" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="23" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="23" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="23" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="23" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="24">
@@ -368,7 +511,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1600"/>
-              <a:t>Sprint Burndown</a:t>
+              <a:t>Project Burndown</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -414,43 +557,43 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Jour 1</c:v>
+                  <c:v>Sprint 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Jour 2</c:v>
+                  <c:v>Sprint 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Jour 3</c:v>
+                  <c:v>Sprint 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Jour 4</c:v>
+                  <c:v>Sprint 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Jour 5</c:v>
+                  <c:v>Sprint 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sprint1!$E$15:$I$15</c:f>
+              <c:f>Sprint1!$E$16:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -540,16 +683,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>285525</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>139411</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>437925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>206086</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>264708</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>139411</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>398058</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>72736</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -856,10 +999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -867,474 +1010,459 @@
     <col min="1" max="1" width="52.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="12" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25"/>
+    </row>
+    <row r="3" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="10">
+        <v>4</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="11" t="s">
+      <c r="B4" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="10">
+        <v>3</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="10">
+        <v>9</v>
+      </c>
+      <c r="E5" s="10">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="F5" s="10">
+        <v>0</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="D6" s="10">
+        <v>2</v>
+      </c>
+      <c r="E6" s="10">
+        <v>2</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="10">
+        <v>5</v>
+      </c>
+      <c r="E7" s="10">
+        <v>5</v>
+      </c>
+      <c r="F7" s="10">
+        <v>5</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0</v>
+      </c>
+      <c r="I7" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="10">
+        <v>3</v>
+      </c>
+      <c r="E8" s="10">
+        <v>3</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="10">
+        <v>3</v>
+      </c>
+      <c r="E9" s="10">
+        <v>3</v>
+      </c>
+      <c r="F9" s="10">
+        <v>3</v>
+      </c>
+      <c r="G9" s="10">
+        <v>3</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0</v>
+      </c>
+      <c r="I9" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="10">
+        <v>8</v>
+      </c>
+      <c r="E10" s="10">
+        <v>8</v>
+      </c>
+      <c r="F10" s="10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="10">
+        <v>8</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="10">
+        <v>8</v>
+      </c>
+      <c r="E11" s="10">
+        <v>8</v>
+      </c>
+      <c r="F11" s="10">
+        <v>8</v>
+      </c>
+      <c r="G11" s="10">
+        <v>8</v>
+      </c>
+      <c r="H11" s="10">
+        <v>2</v>
+      </c>
+      <c r="I11" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="10">
+        <v>10</v>
+      </c>
+      <c r="E12" s="10">
+        <v>10</v>
+      </c>
+      <c r="F12" s="10">
+        <v>10</v>
+      </c>
+      <c r="G12" s="10">
+        <v>10</v>
+      </c>
+      <c r="H12" s="10">
+        <v>5</v>
+      </c>
+      <c r="I12" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="11">
+        <v>8</v>
+      </c>
+      <c r="E13" s="11">
+        <v>8</v>
+      </c>
+      <c r="F13" s="11">
+        <v>8</v>
+      </c>
+      <c r="G13" s="11">
+        <v>8</v>
+      </c>
+      <c r="H13" s="11">
+        <v>8</v>
+      </c>
+      <c r="I13" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="D14" s="11">
+        <v>6</v>
+      </c>
+      <c r="E14" s="11">
+        <v>6</v>
+      </c>
+      <c r="F14" s="11">
+        <v>6</v>
+      </c>
+      <c r="G14" s="11">
+        <v>6</v>
+      </c>
+      <c r="H14" s="11">
+        <v>6</v>
+      </c>
+      <c r="I14" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="10" t="s">
-        <v>8</v>
+      <c r="B15" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="11">
+        <v>5</v>
+      </c>
+      <c r="E15" s="11">
+        <v>5</v>
+      </c>
+      <c r="F15" s="11">
+        <v>5</v>
+      </c>
+      <c r="G15" s="11">
+        <v>5</v>
+      </c>
+      <c r="H15" s="11">
+        <v>5</v>
+      </c>
+      <c r="I15" s="13">
+        <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8">
-        <v>0</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8">
-        <v>0</v>
-      </c>
-      <c r="J5" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8">
-        <v>0</v>
-      </c>
-      <c r="J6" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8">
-        <v>0</v>
-      </c>
-      <c r="J7" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="17"/>
+      <c r="B16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8">
-        <v>0</v>
-      </c>
-      <c r="J8" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8">
-        <v>0</v>
-      </c>
-      <c r="J9" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10">
-        <v>8</v>
-      </c>
-      <c r="E10">
-        <v>8</v>
-      </c>
-      <c r="F10">
-        <v>8</v>
-      </c>
-      <c r="G10">
-        <v>8</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10" s="8">
-        <v>0</v>
-      </c>
-      <c r="J10" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11">
-        <v>8</v>
-      </c>
-      <c r="E11">
-        <v>8</v>
-      </c>
-      <c r="F11">
-        <v>8</v>
-      </c>
-      <c r="G11">
-        <v>8</v>
-      </c>
-      <c r="H11">
-        <v>2</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12">
-        <v>10</v>
-      </c>
-      <c r="G12">
-        <v>10</v>
-      </c>
-      <c r="H12">
-        <v>10</v>
-      </c>
-      <c r="I12" s="1">
-        <v>10</v>
-      </c>
-      <c r="J12" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="1">
-        <v>8</v>
-      </c>
-      <c r="E13" s="1">
-        <v>8</v>
-      </c>
-      <c r="F13" s="1">
-        <v>8</v>
-      </c>
-      <c r="G13" s="1">
-        <v>8</v>
-      </c>
-      <c r="H13" s="1">
-        <v>8</v>
-      </c>
-      <c r="I13" s="1">
-        <v>8</v>
-      </c>
-      <c r="J13" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="1">
-        <v>6</v>
-      </c>
-      <c r="E14" s="1">
-        <v>6</v>
-      </c>
-      <c r="F14" s="1">
-        <v>6</v>
-      </c>
-      <c r="G14" s="1">
-        <v>6</v>
-      </c>
-      <c r="H14" s="1">
-        <v>6</v>
-      </c>
-      <c r="I14" s="1">
-        <v>6</v>
-      </c>
-      <c r="J14" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7">
-        <f>SUM(D3:D14)</f>
-        <v>69</v>
-      </c>
-      <c r="E15" s="12">
-        <f t="shared" ref="E15:J15" si="0">SUM(E3:E14)</f>
-        <v>58</v>
-      </c>
-      <c r="F15" s="12">
+      <c r="C16" s="5"/>
+      <c r="D16" s="22">
+        <f t="shared" ref="D16:I16" si="0">SUM(D3:D15)</f>
+        <v>74</v>
+      </c>
+      <c r="E16" s="7">
         <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="G15" s="12">
+        <v>63</v>
+      </c>
+      <c r="F16" s="7">
         <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="H15" s="12">
+        <v>54</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="H16" s="7">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I16" s="7">
         <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="J15" s="12">
-        <f t="shared" si="0"/>
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>